<commit_message>
ajustes na tabela de dados
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\PQSAnaliseDocumentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D992B679-04BF-483C-B676-50A083FCCAE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86434E9-E695-4DB1-84B4-3925A9C5DD3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{6F00A9CE-EC6D-4C4D-84EE-4C4AF610B84B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Linhas</t>
   </si>
@@ -64,13 +64,23 @@
   </si>
   <si>
     <t>rwasef1830</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,14 +106,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -415,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F31EF94-EE12-4615-A93A-8D697F47BA36}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,33 +444,66 @@
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" ref="D2:D4" si="0">(C2/B2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -464,35 +513,99 @@
       <c r="C5">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <f>(C5/B5)</f>
+        <v>5.7773109243697482E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" ref="D6:D11" si="1">(C6/B6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adição de todos os commits de todos os programadores selecionados
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\PQSAnaliseDocumentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF9CBB1-A404-4206-B071-DB12BEEAFBD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF61F69-4752-4AC8-AC68-CEDD72E495F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{6F00A9CE-EC6D-4C4D-84EE-4C4AF610B84B}"/>
   </bookViews>
@@ -437,7 +437,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,14 +466,14 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>1427</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>254</v>
       </c>
       <c r="D2" s="1">
         <f t="shared" ref="D2:D4" si="0">(C2/B2)</f>
-        <v>1</v>
+        <v>0.17799579537491239</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -481,14 +481,14 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>1001</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8.5914085914085919E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -617,11 +617,11 @@
       </c>
       <c r="B13">
         <f>SUM(B2:B11)</f>
-        <v>2132</v>
+        <v>4558</v>
       </c>
       <c r="C13">
         <f>SUM(C2:C11)</f>
-        <v>83</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
novos relatorios e atualizacao tabela dados
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\PQSAnaliseDocumentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\TrabalhoLesandroPQS\PQSAnaliseDocumentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF61F69-4752-4AC8-AC68-CEDD72E495F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{90BB535A-F7B7-4963-A2D9-A0FC66CE5742}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{6F00A9CE-EC6D-4C4D-84EE-4C4AF610B84B}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +85,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -113,12 +121,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F31EF94-EE12-4615-A93A-8D697F47BA36}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +456,7 @@
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -461,7 +470,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -472,11 +481,11 @@
         <v>254</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D4" si="0">(C2/B2)</f>
+        <f>(C2/B2)</f>
         <v>0.17799579537491239</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -487,11 +496,11 @@
         <v>86</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D2:D4" si="0">(C3/B3)</f>
         <v>8.5914085914085919E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -506,7 +515,7 @@
         <v>2.197802197802198E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -521,7 +530,7 @@
         <v>5.7773109243697482E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -536,95 +545,98 @@
         <v>1.756007393715342E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>308</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9.74025974025974E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>1932</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.9151138716356108E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.3513513513513514E-2</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>576</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13">
         <f>SUM(B2:B11)</f>
-        <v>4558</v>
+        <v>7485</v>
       </c>
       <c r="C13">
         <f>SUM(C2:C11)</f>
-        <v>421</v>
+        <v>466</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>